<commit_message>
fix: naming the index columns in the data excel file
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farha\WorkDirectory\Postdoc\Deployment\Stremlit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farha\WorkDirectory\Postdoc\Deployment\Stremlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0828DF-009C-4E2A-A6AF-2076769CA808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C11F4D-F16A-44CC-A5E2-C1B75CEAEFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>diameter</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>stress_ratio</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -1167,36 +1170,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2911F6C8-E3C9-48AC-BC00-1A07EC7762BC}">
   <dimension ref="A1:V258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A258"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1261,7 +1266,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>0</v>
       </c>
@@ -1333,7 +1338,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -1405,7 +1410,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -1477,7 +1482,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -1549,7 +1554,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -1621,7 +1626,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -1693,7 +1698,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1765,7 +1770,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -1837,7 +1842,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -1909,7 +1914,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -1981,7 +1986,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -2053,7 +2058,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -2125,7 +2130,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -2197,7 +2202,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -2269,7 +2274,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -2341,7 +2346,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -2413,7 +2418,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -2485,7 +2490,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -2557,7 +2562,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -2629,7 +2634,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -2701,7 +2706,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>20</v>
       </c>
@@ -2773,7 +2778,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -2845,7 +2850,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>22</v>
       </c>
@@ -2917,7 +2922,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>23</v>
       </c>
@@ -2989,7 +2994,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>24</v>
       </c>
@@ -3061,7 +3066,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>25</v>
       </c>
@@ -3133,7 +3138,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>26</v>
       </c>
@@ -3205,7 +3210,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -3277,7 +3282,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>28</v>
       </c>
@@ -3349,7 +3354,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>29</v>
       </c>
@@ -3421,7 +3426,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>30</v>
       </c>
@@ -3493,7 +3498,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>31</v>
       </c>
@@ -3565,7 +3570,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>32</v>
       </c>
@@ -3637,7 +3642,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>33</v>
       </c>
@@ -3709,7 +3714,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>34</v>
       </c>
@@ -3781,7 +3786,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>35</v>
       </c>
@@ -3853,7 +3858,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>36</v>
       </c>
@@ -3925,7 +3930,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>37</v>
       </c>
@@ -3997,7 +4002,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>38</v>
       </c>
@@ -4069,7 +4074,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>39</v>
       </c>
@@ -4141,7 +4146,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>40</v>
       </c>
@@ -4213,7 +4218,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>41</v>
       </c>
@@ -4285,7 +4290,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>42</v>
       </c>
@@ -4357,7 +4362,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>43</v>
       </c>
@@ -4412,7 +4417,7 @@
       <c r="U45" s="34"/>
       <c r="V45" s="34"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>44</v>
       </c>
@@ -4467,7 +4472,7 @@
       <c r="U46" s="34"/>
       <c r="V46" s="34"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>45</v>
       </c>
@@ -4539,7 +4544,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>46</v>
       </c>
@@ -4611,7 +4616,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>47</v>
       </c>
@@ -4683,7 +4688,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>48</v>
       </c>
@@ -4755,7 +4760,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>49</v>
       </c>
@@ -4810,7 +4815,7 @@
       <c r="U51" s="34"/>
       <c r="V51" s="34"/>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>50</v>
       </c>
@@ -4882,7 +4887,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>51</v>
       </c>
@@ -4954,7 +4959,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>52</v>
       </c>
@@ -5026,7 +5031,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>53</v>
       </c>
@@ -5098,7 +5103,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>54</v>
       </c>
@@ -5170,7 +5175,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
         <v>55</v>
       </c>
@@ -5242,7 +5247,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="10">
         <v>56</v>
       </c>
@@ -5314,7 +5319,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>57</v>
       </c>
@@ -5386,7 +5391,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
         <v>58</v>
       </c>
@@ -5441,7 +5446,7 @@
       <c r="U60" s="34"/>
       <c r="V60" s="34"/>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
         <v>59</v>
       </c>
@@ -5496,7 +5501,7 @@
       <c r="U61" s="34"/>
       <c r="V61" s="34"/>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="10">
         <v>60</v>
       </c>
@@ -5568,7 +5573,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
         <v>61</v>
       </c>
@@ -5640,7 +5645,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="10">
         <v>62</v>
       </c>
@@ -5712,7 +5717,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="10">
         <v>63</v>
       </c>
@@ -5767,7 +5772,7 @@
       <c r="U65" s="34"/>
       <c r="V65" s="34"/>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
         <v>64</v>
       </c>
@@ -5822,7 +5827,7 @@
       <c r="U66" s="34"/>
       <c r="V66" s="34"/>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
         <v>65</v>
       </c>
@@ -5894,7 +5899,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="10">
         <v>66</v>
       </c>
@@ -5966,7 +5971,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="10">
         <v>67</v>
       </c>
@@ -6038,7 +6043,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="10">
         <v>68</v>
       </c>
@@ -6110,7 +6115,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" s="10">
         <v>69</v>
       </c>
@@ -6182,7 +6187,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="10">
         <v>70</v>
       </c>
@@ -6254,7 +6259,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10">
         <v>71</v>
       </c>
@@ -6326,7 +6331,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="10">
         <v>72</v>
       </c>
@@ -6398,7 +6403,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" s="10">
         <v>73</v>
       </c>
@@ -6470,7 +6475,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="10">
         <v>74</v>
       </c>
@@ -6542,7 +6547,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" s="10">
         <v>75</v>
       </c>
@@ -6614,7 +6619,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" s="10">
         <v>76</v>
       </c>
@@ -6686,7 +6691,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" s="10">
         <v>77</v>
       </c>
@@ -6758,7 +6763,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="10">
         <v>78</v>
       </c>
@@ -6830,7 +6835,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" s="10">
         <v>79</v>
       </c>
@@ -6902,7 +6907,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82" s="10">
         <v>80</v>
       </c>
@@ -6974,7 +6979,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" s="10">
         <v>81</v>
       </c>
@@ -7046,7 +7051,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" s="10">
         <v>82</v>
       </c>
@@ -7118,7 +7123,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A85" s="10">
         <v>83</v>
       </c>
@@ -7190,7 +7195,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A86" s="10">
         <v>84</v>
       </c>
@@ -7262,7 +7267,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A87" s="10">
         <v>85</v>
       </c>
@@ -7334,7 +7339,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" s="10">
         <v>86</v>
       </c>
@@ -7406,7 +7411,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A89" s="10">
         <v>87</v>
       </c>
@@ -7478,7 +7483,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A90" s="10">
         <v>88</v>
       </c>
@@ -7550,7 +7555,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A91" s="10">
         <v>89</v>
       </c>
@@ -7622,7 +7627,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A92" s="10">
         <v>90</v>
       </c>
@@ -7694,7 +7699,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A93" s="10">
         <v>91</v>
       </c>
@@ -7766,7 +7771,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A94" s="10">
         <v>92</v>
       </c>
@@ -7838,7 +7843,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A95" s="10">
         <v>93</v>
       </c>
@@ -7910,7 +7915,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" s="10">
         <v>94</v>
       </c>
@@ -7982,7 +7987,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A97" s="10">
         <v>95</v>
       </c>
@@ -8054,7 +8059,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A98" s="10">
         <v>96</v>
       </c>
@@ -8126,7 +8131,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A99" s="10">
         <v>97</v>
       </c>
@@ -8198,7 +8203,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A100" s="10">
         <v>98</v>
       </c>
@@ -8270,7 +8275,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A101" s="10">
         <v>99</v>
       </c>
@@ -8342,7 +8347,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A102" s="10">
         <v>100</v>
       </c>
@@ -8414,7 +8419,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A103" s="10">
         <v>101</v>
       </c>
@@ -8486,7 +8491,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A104" s="10">
         <v>102</v>
       </c>
@@ -8558,7 +8563,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A105" s="10">
         <v>103</v>
       </c>
@@ -8630,7 +8635,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A106" s="10">
         <v>104</v>
       </c>
@@ -8702,7 +8707,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A107" s="10">
         <v>105</v>
       </c>
@@ -8774,7 +8779,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A108" s="10">
         <v>106</v>
       </c>
@@ -8846,7 +8851,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A109" s="10">
         <v>107</v>
       </c>
@@ -8918,7 +8923,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A110" s="10">
         <v>108</v>
       </c>
@@ -8990,7 +8995,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A111" s="10">
         <v>109</v>
       </c>
@@ -9062,7 +9067,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A112" s="10">
         <v>110</v>
       </c>
@@ -9134,7 +9139,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A113" s="10">
         <v>111</v>
       </c>
@@ -9206,7 +9211,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A114" s="10">
         <v>112</v>
       </c>
@@ -9278,7 +9283,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A115" s="10">
         <v>113</v>
       </c>
@@ -9350,7 +9355,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A116" s="10">
         <v>114</v>
       </c>
@@ -9422,7 +9427,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A117" s="10">
         <v>115</v>
       </c>
@@ -9494,7 +9499,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A118" s="10">
         <v>116</v>
       </c>
@@ -9566,7 +9571,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A119" s="10">
         <v>117</v>
       </c>
@@ -9638,7 +9643,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A120" s="10">
         <v>118</v>
       </c>
@@ -9710,7 +9715,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A121" s="10">
         <v>119</v>
       </c>
@@ -9782,7 +9787,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A122" s="10">
         <v>120</v>
       </c>
@@ -9854,7 +9859,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A123" s="10">
         <v>121</v>
       </c>
@@ -9926,7 +9931,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A124" s="10">
         <v>122</v>
       </c>
@@ -9998,7 +10003,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A125" s="10">
         <v>123</v>
       </c>
@@ -10070,7 +10075,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A126" s="10">
         <v>124</v>
       </c>
@@ -10142,7 +10147,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A127" s="10">
         <v>125</v>
       </c>
@@ -10214,7 +10219,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A128" s="10">
         <v>126</v>
       </c>
@@ -10286,7 +10291,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A129" s="10">
         <v>127</v>
       </c>
@@ -10358,7 +10363,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A130" s="10">
         <v>128</v>
       </c>
@@ -10430,7 +10435,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A131" s="10">
         <v>129</v>
       </c>
@@ -10502,7 +10507,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A132" s="10">
         <v>130</v>
       </c>
@@ -10574,7 +10579,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A133" s="10">
         <v>131</v>
       </c>
@@ -10646,7 +10651,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A134" s="10">
         <v>132</v>
       </c>
@@ -10718,7 +10723,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A135" s="10">
         <v>133</v>
       </c>
@@ -10790,7 +10795,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A136" s="10">
         <v>134</v>
       </c>
@@ -10862,7 +10867,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A137" s="10">
         <v>135</v>
       </c>
@@ -10934,7 +10939,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A138" s="10">
         <v>136</v>
       </c>
@@ -11006,7 +11011,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A139" s="10">
         <v>137</v>
       </c>
@@ -11078,7 +11083,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A140" s="10">
         <v>138</v>
       </c>
@@ -11150,7 +11155,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A141" s="10">
         <v>139</v>
       </c>
@@ -11222,7 +11227,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A142" s="10">
         <v>140</v>
       </c>
@@ -11294,7 +11299,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A143" s="10">
         <v>141</v>
       </c>
@@ -11366,7 +11371,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A144" s="10">
         <v>142</v>
       </c>
@@ -11438,7 +11443,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A145" s="10">
         <v>143</v>
       </c>
@@ -11510,7 +11515,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="146" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="10">
         <v>144</v>
       </c>
@@ -11583,7 +11588,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="147" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="10">
         <v>145</v>
       </c>
@@ -11656,7 +11661,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="148" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="10">
         <v>146</v>
       </c>
@@ -11729,7 +11734,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="149" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="10">
         <v>147</v>
       </c>
@@ -11802,7 +11807,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="150" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="10">
         <v>148</v>
       </c>
@@ -11875,7 +11880,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="151" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="10">
         <v>149</v>
       </c>
@@ -11948,7 +11953,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="152" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="10">
         <v>150</v>
       </c>
@@ -12021,7 +12026,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="153" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="10">
         <v>151</v>
       </c>
@@ -12094,7 +12099,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="154" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="10">
         <v>152</v>
       </c>
@@ -12167,7 +12172,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="155" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="10">
         <v>153</v>
       </c>
@@ -12240,7 +12245,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="156" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="10">
         <v>154</v>
       </c>
@@ -12313,7 +12318,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="157" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="10">
         <v>155</v>
       </c>
@@ -12386,7 +12391,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="158" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="10">
         <v>156</v>
       </c>
@@ -12459,7 +12464,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="159" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="10">
         <v>157</v>
       </c>
@@ -12532,7 +12537,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="160" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="10">
         <v>158</v>
       </c>
@@ -12605,7 +12610,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="161" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="10">
         <v>159</v>
       </c>
@@ -12678,7 +12683,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="162" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="10">
         <v>160</v>
       </c>
@@ -12751,7 +12756,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="163" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="10">
         <v>161</v>
       </c>
@@ -12824,7 +12829,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="164" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="10">
         <v>162</v>
       </c>
@@ -12897,7 +12902,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="165" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="10">
         <v>163</v>
       </c>
@@ -12970,7 +12975,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="166" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="10">
         <v>164</v>
       </c>
@@ -13043,7 +13048,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="167" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="10">
         <v>165</v>
       </c>
@@ -13116,7 +13121,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="168" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="10">
         <v>166</v>
       </c>
@@ -13189,7 +13194,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="169" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="10">
         <v>167</v>
       </c>
@@ -13262,7 +13267,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="170" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="10">
         <v>168</v>
       </c>
@@ -13335,7 +13340,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="171" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="10">
         <v>169</v>
       </c>
@@ -13408,7 +13413,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="172" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="10">
         <v>170</v>
       </c>
@@ -13481,7 +13486,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="173" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="10">
         <v>171</v>
       </c>
@@ -13554,7 +13559,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="174" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="10">
         <v>172</v>
       </c>
@@ -13627,7 +13632,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="175" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="10">
         <v>173</v>
       </c>
@@ -13700,7 +13705,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="176" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="10">
         <v>174</v>
       </c>
@@ -13773,7 +13778,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="177" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="10">
         <v>175</v>
       </c>
@@ -13846,7 +13851,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="178" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="10">
         <v>176</v>
       </c>
@@ -13919,7 +13924,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="179" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="10">
         <v>177</v>
       </c>
@@ -13992,7 +13997,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="180" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="10">
         <v>178</v>
       </c>
@@ -14065,7 +14070,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="181" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="10">
         <v>179</v>
       </c>
@@ -14138,7 +14143,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="182" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="10">
         <v>180</v>
       </c>
@@ -14211,7 +14216,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="183" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="10">
         <v>181</v>
       </c>
@@ -14284,7 +14289,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="184" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="10">
         <v>182</v>
       </c>
@@ -14357,7 +14362,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="185" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="10">
         <v>183</v>
       </c>
@@ -14430,7 +14435,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="186" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="10">
         <v>184</v>
       </c>
@@ -14503,7 +14508,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="187" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="10">
         <v>185</v>
       </c>
@@ -14576,7 +14581,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="188" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="10">
         <v>186</v>
       </c>
@@ -14649,7 +14654,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="189" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="10">
         <v>187</v>
       </c>
@@ -14722,7 +14727,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="190" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="10">
         <v>188</v>
       </c>
@@ -14795,7 +14800,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="191" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="10">
         <v>189</v>
       </c>
@@ -14868,7 +14873,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="192" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="10">
         <v>190</v>
       </c>
@@ -14941,7 +14946,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="193" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="10">
         <v>191</v>
       </c>
@@ -15014,7 +15019,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="194" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="10">
         <v>192</v>
       </c>
@@ -15087,7 +15092,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="195" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="10">
         <v>193</v>
       </c>
@@ -15160,7 +15165,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="196" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="10">
         <v>194</v>
       </c>
@@ -15233,7 +15238,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="197" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="10">
         <v>195</v>
       </c>
@@ -15306,7 +15311,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="198" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="10">
         <v>196</v>
       </c>
@@ -15379,7 +15384,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="199" spans="1:22" s="10" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:22" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="10">
         <v>197</v>
       </c>
@@ -15452,7 +15457,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="200" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="10">
         <v>198</v>
       </c>
@@ -15525,7 +15530,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="201" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="10">
         <v>199</v>
       </c>
@@ -15598,7 +15603,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="202" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="10">
         <v>200</v>
       </c>
@@ -15671,7 +15676,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="203" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="10">
         <v>201</v>
       </c>
@@ -15743,7 +15748,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="204" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="10">
         <v>202</v>
       </c>
@@ -15815,7 +15820,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="205" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="10">
         <v>203</v>
       </c>
@@ -15888,7 +15893,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="206" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="10">
         <v>204</v>
       </c>
@@ -15961,7 +15966,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="207" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="10">
         <v>205</v>
       </c>
@@ -16034,7 +16039,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="208" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="10">
         <v>206</v>
       </c>
@@ -16106,7 +16111,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="209" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="10">
         <v>207</v>
       </c>
@@ -16179,7 +16184,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="210" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="10">
         <v>208</v>
       </c>
@@ -16252,7 +16257,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="211" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="10">
         <v>209</v>
       </c>
@@ -16307,7 +16312,7 @@
       <c r="U211" s="35"/>
       <c r="V211" s="35"/>
     </row>
-    <row r="212" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="10">
         <v>210</v>
       </c>
@@ -16380,7 +16385,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="213" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="10">
         <v>211</v>
       </c>
@@ -16453,7 +16458,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="214" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="10">
         <v>212</v>
       </c>
@@ -16525,7 +16530,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="215" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="10">
         <v>213</v>
       </c>
@@ -16598,7 +16603,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="216" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="10">
         <v>214</v>
       </c>
@@ -16671,7 +16676,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="217" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="10">
         <v>215</v>
       </c>
@@ -16744,7 +16749,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="218" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="10">
         <v>216</v>
       </c>
@@ -16817,7 +16822,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="219" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="10">
         <v>217</v>
       </c>
@@ -16889,7 +16894,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="220" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="10">
         <v>218</v>
       </c>
@@ -16962,7 +16967,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="221" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="10">
         <v>219</v>
       </c>
@@ -17035,7 +17040,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="222" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="10">
         <v>220</v>
       </c>
@@ -17107,7 +17112,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="223" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="10">
         <v>221</v>
       </c>
@@ -17180,7 +17185,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="224" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="10">
         <v>222</v>
       </c>
@@ -17253,7 +17258,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="225" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="10">
         <v>223</v>
       </c>
@@ -17326,7 +17331,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="226" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="10">
         <v>224</v>
       </c>
@@ -17399,7 +17404,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="227" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="10">
         <v>225</v>
       </c>
@@ -17471,7 +17476,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="228" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="10">
         <v>226</v>
       </c>
@@ -17544,7 +17549,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="229" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="10">
         <v>227</v>
       </c>
@@ -17617,7 +17622,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="230" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="10">
         <v>228</v>
       </c>
@@ -17690,7 +17695,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="231" spans="1:22" s="10" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:22" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="10">
         <v>229</v>
       </c>
@@ -17763,7 +17768,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="232" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A232" s="10">
         <v>230</v>
       </c>
@@ -17836,7 +17841,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="233" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="10">
         <v>231</v>
       </c>
@@ -17908,7 +17913,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="234" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="10">
         <v>232</v>
       </c>
@@ -17981,7 +17986,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="235" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="10">
         <v>233</v>
       </c>
@@ -18054,7 +18059,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="236" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A236" s="10">
         <v>234</v>
       </c>
@@ -18127,7 +18132,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="237" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="10">
         <v>235</v>
       </c>
@@ -18200,7 +18205,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="238" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="10">
         <v>236</v>
       </c>
@@ -18272,7 +18277,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="239" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A239" s="10">
         <v>237</v>
       </c>
@@ -18345,7 +18350,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="240" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A240" s="10">
         <v>238</v>
       </c>
@@ -18418,7 +18423,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="241" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A241" s="10">
         <v>239</v>
       </c>
@@ -18491,7 +18496,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="242" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A242" s="10">
         <v>240</v>
       </c>
@@ -18564,7 +18569,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="243" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A243" s="10">
         <v>241</v>
       </c>
@@ -18637,7 +18642,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="244" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A244" s="10">
         <v>242</v>
       </c>
@@ -18710,7 +18715,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="245" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A245" s="10">
         <v>243</v>
       </c>
@@ -18782,7 +18787,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="246" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A246" s="10">
         <v>244</v>
       </c>
@@ -18855,7 +18860,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="247" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A247" s="10">
         <v>245</v>
       </c>
@@ -18928,7 +18933,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="248" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A248" s="10">
         <v>246</v>
       </c>
@@ -19001,7 +19006,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="249" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A249" s="10">
         <v>247</v>
       </c>
@@ -19074,7 +19079,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="250" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A250" s="10">
         <v>248</v>
       </c>
@@ -19147,7 +19152,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="251" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A251" s="10">
         <v>249</v>
       </c>
@@ -19219,7 +19224,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="252" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A252" s="10">
         <v>250</v>
       </c>
@@ -19292,7 +19297,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="253" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="10">
         <v>251</v>
       </c>
@@ -19365,7 +19370,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="254" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A254" s="10">
         <v>252</v>
       </c>
@@ -19438,7 +19443,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="255" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A255" s="10">
         <v>253</v>
       </c>
@@ -19511,7 +19516,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="256" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A256" s="10">
         <v>254</v>
       </c>
@@ -19583,7 +19588,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="257" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A257" s="10">
         <v>255</v>
       </c>
@@ -19656,7 +19661,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="258" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" s="10">
         <v>256</v>
       </c>
@@ -19742,31 +19747,31 @@
       <selection activeCell="A2" sqref="A2:XFD73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="16" t="s">
         <v>0</v>
@@ -19832,7 +19837,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>0</v>
       </c>
@@ -19904,7 +19909,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -19976,7 +19981,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -20048,7 +20053,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>2</v>
       </c>
@@ -20120,7 +20125,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>0</v>
       </c>
@@ -20192,7 +20197,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>1</v>
       </c>
@@ -20264,7 +20269,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>2</v>
       </c>
@@ -20336,7 +20341,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>2</v>
       </c>
@@ -20408,7 +20413,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>3</v>
       </c>
@@ -20480,7 +20485,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>4</v>
       </c>
@@ -20552,7 +20557,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>5</v>
       </c>
@@ -20624,7 +20629,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>5</v>
       </c>
@@ -20696,7 +20701,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>6</v>
       </c>
@@ -20768,7 +20773,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>7</v>
       </c>
@@ -20840,7 +20845,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>8</v>
       </c>
@@ -20912,7 +20917,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>9</v>
       </c>
@@ -20984,7 +20989,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>9</v>
       </c>
@@ -21056,7 +21061,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>6</v>
       </c>
@@ -21128,7 +21133,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>7</v>
       </c>
@@ -21200,7 +21205,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>8</v>
       </c>
@@ -21272,7 +21277,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>9</v>
       </c>
@@ -21344,7 +21349,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>9</v>
       </c>
@@ -21416,7 +21421,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>10</v>
       </c>
@@ -21488,7 +21493,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>11</v>
       </c>
@@ -21560,7 +21565,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>12</v>
       </c>
@@ -21632,7 +21637,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>13</v>
       </c>
@@ -21704,7 +21709,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>13</v>
       </c>
@@ -21776,7 +21781,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>14</v>
       </c>
@@ -21848,7 +21853,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>15</v>
       </c>
@@ -21920,7 +21925,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>16</v>
       </c>
@@ -21992,7 +21997,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>17</v>
       </c>
@@ -22064,7 +22069,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>17</v>
       </c>
@@ -22136,7 +22141,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>14</v>
       </c>
@@ -22208,7 +22213,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>15</v>
       </c>
@@ -22280,7 +22285,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>16</v>
       </c>
@@ -22352,7 +22357,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>17</v>
       </c>
@@ -22424,7 +22429,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>17</v>
       </c>
@@ -22496,7 +22501,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>18</v>
       </c>
@@ -22568,7 +22573,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>19</v>
       </c>
@@ -22640,7 +22645,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>19</v>
       </c>
@@ -22712,7 +22717,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>20</v>
       </c>
@@ -22784,7 +22789,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>20</v>
       </c>
@@ -22856,7 +22861,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>21</v>
       </c>
@@ -22928,7 +22933,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>21</v>
       </c>
@@ -22996,7 +23001,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>21</v>
       </c>
@@ -23064,7 +23069,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>24</v>
       </c>
@@ -23136,7 +23141,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>24</v>
       </c>
@@ -23208,7 +23213,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>21</v>
       </c>
@@ -23280,7 +23285,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>23</v>
       </c>
@@ -23352,7 +23357,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>23</v>
       </c>
@@ -23420,7 +23425,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>23</v>
       </c>
@@ -23492,7 +23497,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>24</v>
       </c>
@@ -23564,7 +23569,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>24</v>
       </c>
@@ -23636,7 +23641,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>25</v>
       </c>
@@ -23708,7 +23713,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>26</v>
       </c>
@@ -23780,7 +23785,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
         <v>27</v>
       </c>
@@ -23852,7 +23857,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="10">
         <v>27</v>
       </c>
@@ -23924,7 +23929,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>28</v>
       </c>
@@ -23996,7 +24001,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
         <v>30</v>
       </c>
@@ -24064,7 +24069,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
         <v>30</v>
       </c>
@@ -24132,7 +24137,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="10">
         <v>31</v>
       </c>
@@ -24204,7 +24209,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
         <v>31</v>
       </c>
@@ -24276,7 +24281,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="10">
         <v>28</v>
       </c>
@@ -24348,7 +24353,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="10">
         <v>30</v>
       </c>
@@ -24416,7 +24421,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
         <v>30</v>
       </c>
@@ -24484,7 +24489,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
         <v>31</v>
       </c>
@@ -24556,7 +24561,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="10">
         <v>31</v>
       </c>
@@ -24628,7 +24633,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="10">
         <v>32</v>
       </c>
@@ -24700,7 +24705,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="10">
         <v>33</v>
       </c>
@@ -24772,7 +24777,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" s="10">
         <v>34</v>
       </c>
@@ -24844,7 +24849,7 @@
         <v>431.2</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="10">
         <v>35</v>
       </c>
@@ -24916,7 +24921,7 @@
         <v>424.9</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" s="10">
         <v>35</v>
       </c>
@@ -24988,7 +24993,7 @@
         <v>418.6</v>
       </c>
     </row>
-    <row r="177" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A177" s="10"/>
       <c r="B177" s="7"/>
       <c r="C177" s="3"/>
@@ -25012,10 +25017,10 @@
       <c r="U177" s="14"/>
       <c r="V177" s="14"/>
     </row>
-    <row r="206" spans="20:20" x14ac:dyDescent="0.3">
+    <row r="206" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T206" s="9"/>
     </row>
-    <row r="207" spans="20:20" x14ac:dyDescent="0.3">
+    <row r="207" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T207" s="9"/>
     </row>
   </sheetData>
@@ -25032,12 +25037,12 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10">
         <v>36</v>
       </c>
@@ -25109,7 +25114,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>37</v>
       </c>
@@ -25181,7 +25186,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>38</v>
       </c>
@@ -25253,7 +25258,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>39</v>
       </c>
@@ -25325,7 +25330,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>40</v>
       </c>
@@ -25397,7 +25402,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>41</v>
       </c>
@@ -25469,7 +25474,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>42</v>
       </c>
@@ -25541,7 +25546,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="10" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="10" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>43</v>
       </c>
@@ -25613,7 +25618,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>44</v>
       </c>
@@ -25685,7 +25690,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>45</v>
       </c>
@@ -25757,7 +25762,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>46</v>
       </c>
@@ -25829,7 +25834,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>47</v>
       </c>
@@ -25901,7 +25906,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>48</v>
       </c>
@@ -25973,7 +25978,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>49</v>
       </c>
@@ -26045,7 +26050,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>50</v>
       </c>
@@ -26117,7 +26122,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>51</v>
       </c>
@@ -26189,7 +26194,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>51</v>
       </c>
@@ -26261,7 +26266,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>54</v>
       </c>
@@ -26333,7 +26338,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>53</v>
       </c>
@@ -26405,7 +26410,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="20" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>52</v>
       </c>
@@ -26477,7 +26482,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>59</v>
       </c>
@@ -26549,7 +26554,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>60</v>
       </c>
@@ -26621,7 +26626,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>61</v>
       </c>
@@ -26693,7 +26698,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>62</v>
       </c>
@@ -26765,7 +26770,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>41</v>
       </c>
@@ -26837,7 +26842,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="26" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>41</v>
       </c>
@@ -26909,7 +26914,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="27" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>41</v>
       </c>
@@ -26981,7 +26986,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="28" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>63</v>
       </c>
@@ -27053,7 +27058,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>64</v>
       </c>
@@ -27125,7 +27130,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="30" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>65</v>
       </c>
@@ -27197,7 +27202,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="31" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>66</v>
       </c>
@@ -27269,7 +27274,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="32" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>67</v>
       </c>
@@ -27341,7 +27346,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="33" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>68</v>
       </c>
@@ -27411,7 +27416,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="34" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>69</v>
       </c>
@@ -27483,7 +27488,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>70</v>
       </c>
@@ -27555,7 +27560,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="36" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>71</v>
       </c>
@@ -27627,7 +27632,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="37" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>72</v>
       </c>
@@ -27699,7 +27704,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="38" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>73</v>
       </c>
@@ -27771,7 +27776,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="39" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>74</v>
       </c>
@@ -27843,7 +27848,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="40" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>75</v>
       </c>
@@ -27915,7 +27920,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="41" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>76</v>
       </c>
@@ -27987,7 +27992,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="42" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>77</v>
       </c>
@@ -28059,7 +28064,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="43" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>78</v>
       </c>
@@ -28131,7 +28136,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="44" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>79</v>
       </c>
@@ -28203,7 +28208,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>80</v>
       </c>
@@ -28275,7 +28280,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="46" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>81</v>
       </c>
@@ -28347,7 +28352,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>82</v>
       </c>
@@ -28419,7 +28424,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="48" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>82</v>
       </c>
@@ -28491,7 +28496,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="49" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>83</v>
       </c>
@@ -28563,7 +28568,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="50" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>84</v>
       </c>
@@ -28635,7 +28640,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="51" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>85</v>
       </c>
@@ -28707,7 +28712,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="52" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>86</v>
       </c>
@@ -28779,7 +28784,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="53" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>86</v>
       </c>
@@ -28851,7 +28856,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="54" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>87</v>
       </c>
@@ -28923,7 +28928,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="55" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>87</v>
       </c>
@@ -28995,7 +29000,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="56" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>88</v>
       </c>
@@ -29067,7 +29072,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="57" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
         <v>88</v>
       </c>
@@ -29139,7 +29144,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="58" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10">
         <v>89</v>
       </c>
@@ -29211,7 +29216,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="59" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>89</v>
       </c>
@@ -29283,7 +29288,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="60" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
         <v>90</v>
       </c>
@@ -29355,7 +29360,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="61" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
         <v>90</v>
       </c>
@@ -29427,7 +29432,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="62" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10">
         <v>90</v>
       </c>
@@ -29499,7 +29504,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="63" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
         <v>90</v>
       </c>
@@ -29571,7 +29576,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="64" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10">
         <v>63</v>
       </c>
@@ -29643,7 +29648,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="65" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10">
         <v>63</v>
       </c>
@@ -29715,7 +29720,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="66" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
         <v>63</v>
       </c>
@@ -29787,7 +29792,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="67" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
         <v>91</v>
       </c>
@@ -29859,7 +29864,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="68" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10">
         <v>92</v>
       </c>
@@ -29931,7 +29936,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="69" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10">
         <v>93</v>
       </c>
@@ -30003,7 +30008,7 @@
         <v>395.4</v>
       </c>
     </row>
-    <row r="70" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10">
         <v>93</v>
       </c>
@@ -30075,7 +30080,7 @@
         <v>381.3</v>
       </c>
     </row>
-    <row r="71" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10">
         <v>89</v>
       </c>
@@ -30147,7 +30152,7 @@
         <v>408.1</v>
       </c>
     </row>
-    <row r="72" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10">
         <v>81</v>
       </c>
@@ -30232,9 +30237,9 @@
       <selection sqref="A1:XFD57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10">
         <v>94</v>
       </c>
@@ -30307,7 +30312,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>95</v>
       </c>
@@ -30380,7 +30385,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>96</v>
       </c>
@@ -30453,7 +30458,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>97</v>
       </c>
@@ -30526,7 +30531,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>97</v>
       </c>
@@ -30599,7 +30604,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>98</v>
       </c>
@@ -30672,7 +30677,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>99</v>
       </c>
@@ -30745,7 +30750,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>100</v>
       </c>
@@ -30818,7 +30823,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>101</v>
       </c>
@@ -30891,7 +30896,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>101</v>
       </c>
@@ -30964,7 +30969,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>102</v>
       </c>
@@ -31037,7 +31042,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>103</v>
       </c>
@@ -31110,7 +31115,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>104</v>
       </c>
@@ -31183,7 +31188,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>105</v>
       </c>
@@ -31256,7 +31261,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>105</v>
       </c>
@@ -31329,7 +31334,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="10" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="10" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>106</v>
       </c>
@@ -31402,7 +31407,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>107</v>
       </c>
@@ -31475,7 +31480,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>108</v>
       </c>
@@ -31548,7 +31553,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>108</v>
       </c>
@@ -31615,7 +31620,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="20" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>108</v>
       </c>
@@ -31688,7 +31693,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>109</v>
       </c>
@@ -31761,7 +31766,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>110</v>
       </c>
@@ -31834,7 +31839,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>111</v>
       </c>
@@ -31907,7 +31912,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>112</v>
       </c>
@@ -31980,7 +31985,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>112</v>
       </c>
@@ -32053,7 +32058,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="26" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>113</v>
       </c>
@@ -32126,7 +32131,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="27" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>114</v>
       </c>
@@ -32199,7 +32204,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="28" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>115</v>
       </c>
@@ -32272,7 +32277,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>116</v>
       </c>
@@ -32345,7 +32350,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="30" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>116</v>
       </c>
@@ -32418,7 +32423,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="31" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>117</v>
       </c>
@@ -32491,7 +32496,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="32" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>118</v>
       </c>
@@ -32564,7 +32569,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="33" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>119</v>
       </c>
@@ -32637,7 +32642,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="34" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>120</v>
       </c>
@@ -32710,7 +32715,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>120</v>
       </c>
@@ -32783,7 +32788,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="36" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>121</v>
       </c>
@@ -32856,7 +32861,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="37" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>122</v>
       </c>
@@ -32929,7 +32934,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="38" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>123</v>
       </c>
@@ -33002,7 +33007,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="39" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>124</v>
       </c>
@@ -33075,7 +33080,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="40" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>124</v>
       </c>
@@ -33148,7 +33153,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="41" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>125</v>
       </c>
@@ -33221,7 +33226,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="42" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>126</v>
       </c>
@@ -33294,7 +33299,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="43" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>127</v>
       </c>
@@ -33367,7 +33372,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="44" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>129</v>
       </c>
@@ -33440,7 +33445,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>129</v>
       </c>
@@ -33513,7 +33518,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="46" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>130</v>
       </c>
@@ -33586,7 +33591,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="47" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>131</v>
       </c>
@@ -33659,7 +33664,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="48" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>132</v>
       </c>
@@ -33732,7 +33737,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="49" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>132</v>
       </c>
@@ -33805,7 +33810,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="50" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>133</v>
       </c>
@@ -33878,7 +33883,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="51" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>134</v>
       </c>
@@ -33951,7 +33956,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="52" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>135</v>
       </c>
@@ -34024,7 +34029,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="53" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>135</v>
       </c>
@@ -34097,7 +34102,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="54" spans="1:22" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" s="2" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>136</v>
       </c>
@@ -34170,7 +34175,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="55" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>137</v>
       </c>
@@ -34243,7 +34248,7 @@
         <v>395.3</v>
       </c>
     </row>
-    <row r="56" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>138</v>
       </c>
@@ -34316,7 +34321,7 @@
         <v>381.8</v>
       </c>
     </row>
-    <row r="57" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
         <v>138</v>
       </c>
@@ -34402,12 +34407,12 @@
       <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="16" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10">
         <v>139</v>
       </c>
@@ -34479,7 +34484,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>153</v>
       </c>
@@ -34551,7 +34556,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>154</v>
       </c>
@@ -34624,7 +34629,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>155</v>
       </c>
@@ -34697,7 +34702,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>156</v>
       </c>
@@ -34770,7 +34775,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>157</v>
       </c>
@@ -34843,7 +34848,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>153</v>
       </c>
@@ -34915,7 +34920,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>154</v>
       </c>
@@ -34988,7 +34993,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>155</v>
       </c>
@@ -35061,7 +35066,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>156</v>
       </c>
@@ -35134,7 +35139,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>157</v>
       </c>
@@ -35207,7 +35212,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>158</v>
       </c>
@@ -35280,7 +35285,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>159</v>
       </c>
@@ -35352,7 +35357,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>160</v>
       </c>
@@ -35425,7 +35430,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>161</v>
       </c>
@@ -35498,7 +35503,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>162</v>
       </c>
@@ -35571,7 +35576,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>163</v>
       </c>
@@ -35644,7 +35649,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>164</v>
       </c>
@@ -35714,7 +35719,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>165</v>
       </c>
@@ -35787,7 +35792,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="20" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>166</v>
       </c>
@@ -35860,7 +35865,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>153</v>
       </c>
@@ -35932,7 +35937,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>154</v>
       </c>
@@ -36005,7 +36010,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>155</v>
       </c>
@@ -36078,7 +36083,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>156</v>
       </c>
@@ -36151,7 +36156,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>157</v>
       </c>
@@ -36224,7 +36229,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="26" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>153</v>
       </c>
@@ -36296,7 +36301,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="27" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>154</v>
       </c>
@@ -36369,7 +36374,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="28" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>155</v>
       </c>
@@ -36442,7 +36447,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>156</v>
       </c>
@@ -36515,7 +36520,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="30" spans="1:22" s="10" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>157</v>
       </c>
@@ -36588,7 +36593,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="31" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>158</v>
       </c>
@@ -36661,7 +36666,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="32" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>159</v>
       </c>
@@ -36733,7 +36738,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="33" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>160</v>
       </c>
@@ -36806,7 +36811,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="34" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>161</v>
       </c>
@@ -36879,7 +36884,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>148</v>
       </c>
@@ -36952,7 +36957,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="36" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>163</v>
       </c>
@@ -37025,7 +37030,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="37" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>164</v>
       </c>
@@ -37097,7 +37102,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="38" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>165</v>
       </c>
@@ -37170,7 +37175,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="39" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>166</v>
       </c>
@@ -37243,7 +37248,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>140</v>
       </c>
@@ -37316,7 +37321,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="41" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>141</v>
       </c>
@@ -37389,7 +37394,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="42" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>142</v>
       </c>
@@ -37462,7 +37467,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="43" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>143</v>
       </c>
@@ -37535,7 +37540,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="44" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>139</v>
       </c>
@@ -37607,7 +37612,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="45" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>140</v>
       </c>
@@ -37680,7 +37685,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="46" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>141</v>
       </c>
@@ -37753,7 +37758,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="47" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>142</v>
       </c>
@@ -37826,7 +37831,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="48" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>143</v>
       </c>
@@ -37899,7 +37904,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="49" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>144</v>
       </c>
@@ -37972,7 +37977,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="50" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>145</v>
       </c>
@@ -38044,7 +38049,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="51" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>146</v>
       </c>
@@ -38117,7 +38122,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="52" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>147</v>
       </c>
@@ -38190,7 +38195,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="53" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>162</v>
       </c>
@@ -38263,7 +38268,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="54" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>149</v>
       </c>
@@ -38336,7 +38341,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="55" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>150</v>
       </c>
@@ -38408,7 +38413,7 @@
         <v>371.2</v>
       </c>
     </row>
-    <row r="56" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>151</v>
       </c>
@@ -38481,7 +38486,7 @@
         <v>357.3</v>
       </c>
     </row>
-    <row r="57" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
         <v>152</v>
       </c>
@@ -38554,7 +38559,7 @@
         <v>379.6</v>
       </c>
     </row>
-    <row r="58" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="12"/>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
@@ -38577,7 +38582,7 @@
       <c r="U58" s="15"/>
       <c r="V58" s="15"/>
     </row>
-    <row r="59" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>

</xml_diff>